<commit_message>
completed 9 test cases for ESPN.com on locating soccer teams, created astest package for mma and detailed test cases in ESPNTests.txt file
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data.xlsx
+++ b/com.espn/src/test/resources/test_data.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.automationpractice\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{267B17A9-AA7E-4FC1-94D0-E3000F6F0E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4E43BB-E7BE-4819-B028-C1B88D2847A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SoccerPage" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,12 +35,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Assertions</t>
   </si>
   <si>
-    <t>WOMEN &gt; COLOR BLACK</t>
+    <t>REAL MADRID</t>
+  </si>
+  <si>
+    <t>PARIS SAINT-GERMAIN</t>
+  </si>
+  <si>
+    <t>MANCHESTER UNITED</t>
+  </si>
+  <si>
+    <t>MANCHESTER CITY</t>
+  </si>
+  <si>
+    <t>JUVENTUS</t>
+  </si>
+  <si>
+    <t>BAYERN MUNICH</t>
+  </si>
+  <si>
+    <t>BARCELONA</t>
+  </si>
+  <si>
+    <t>LIVERPOOL</t>
+  </si>
+  <si>
+    <t>BORUSSIA DORTMUND</t>
   </si>
 </sst>
 </file>
@@ -392,13 +416,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -410,6 +437,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
created test cases to retrive stats and team info
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data.xlsx
+++ b/com.espn/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4E43BB-E7BE-4819-B028-C1B88D2847A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD641C67-7100-43C3-ACC8-6BDA91DABD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="SoccerPage" sheetId="1" r:id="rId1"/>
+    <sheet name="TeamInfo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Assertions</t>
   </si>
@@ -65,6 +66,24 @@
   </si>
   <si>
     <t>BORUSSIA DORTMUND</t>
+  </si>
+  <si>
+    <t>Real Madrid Performance Stats</t>
+  </si>
+  <si>
+    <t>Real Madrid Discipline Stats</t>
+  </si>
+  <si>
+    <t>Real Madrid Scoring Stats</t>
+  </si>
+  <si>
+    <t>Real Madrid Results</t>
+  </si>
+  <si>
+    <t>Real Madrid Squad</t>
+  </si>
+  <si>
+    <t>Real Madrid Transfers</t>
   </si>
 </sst>
 </file>
@@ -418,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -480,4 +499,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5560932B-44D8-4B35-91B4-F602F04E2224}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test cases to ESPN.
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data.xlsx
+++ b/com.espn/src/test/resources/test_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD641C67-7100-43C3-ACC8-6BDA91DABD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A42A6FC-5984-45F4-B1F8-BE67565344B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" activeTab="2" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="SoccerPage" sheetId="1" r:id="rId1"/>
     <sheet name="TeamInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="MMA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Assertions</t>
   </si>
@@ -84,6 +85,33 @@
   </si>
   <si>
     <t>Real Madrid Transfers</t>
+  </si>
+  <si>
+    <t>ARSENAL</t>
+  </si>
+  <si>
+    <t>TOTTENHAM HOTSPUR</t>
+  </si>
+  <si>
+    <t>Paris Saint-Germain Performance Stats</t>
+  </si>
+  <si>
+    <t>Paris Saint-Germain Discipline Stats</t>
+  </si>
+  <si>
+    <t>Paris Saint-Germain Scoring Stats</t>
+  </si>
+  <si>
+    <t>Paris Saint-Germain Results</t>
+  </si>
+  <si>
+    <t>Paris Saint-Germain Squad</t>
+  </si>
+  <si>
+    <t>Paris Saint-Germain Transfers</t>
+  </si>
+  <si>
+    <t>Current and all-time UFC champions</t>
   </si>
 </sst>
 </file>
@@ -119,8 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,6 +527,16 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -503,15 +544,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5560932B-44D8-4B35-91B4-F602F04E2224}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -549,6 +588,62 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA85EE8-E8FA-47DA-86F8-FAC062E4629B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created test cases for the NBA page in espn.
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data.xlsx
+++ b/com.espn/src/test/resources/test_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A42A6FC-5984-45F4-B1F8-BE67565344B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A8104B-970A-4CC3-8136-C0611F92CDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" activeTab="2" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" activeTab="3" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="SoccerPage" sheetId="1" r:id="rId1"/>
     <sheet name="TeamInfo" sheetId="2" r:id="rId2"/>
     <sheet name="MMA" sheetId="3" r:id="rId3"/>
+    <sheet name="NBA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Assertions</t>
   </si>
@@ -112,16 +113,143 @@
   </si>
   <si>
     <t>Current and all-time UFC champions</t>
+  </si>
+  <si>
+    <t>ATLANTA
+HAWKS</t>
+  </si>
+  <si>
+    <t>BOSTON
+CELTICS</t>
+  </si>
+  <si>
+    <t>BROOKLYN
+NETS</t>
+  </si>
+  <si>
+    <t>CHARLOTTE
+HORNETS</t>
+  </si>
+  <si>
+    <t>CHICAGO
+BULLS</t>
+  </si>
+  <si>
+    <t>CLEVELAND
+CAVALIERS</t>
+  </si>
+  <si>
+    <t>DALLAS
+MAVERICKS</t>
+  </si>
+  <si>
+    <t>DENVER
+NUGGETS</t>
+  </si>
+  <si>
+    <t>DETROIT
+PISTONS</t>
+  </si>
+  <si>
+    <t>GOLDEN STATE
+WARRIORS</t>
+  </si>
+  <si>
+    <t>HOUSTON
+ROCKETS</t>
+  </si>
+  <si>
+    <t>INDIANA
+PACERS</t>
+  </si>
+  <si>
+    <t>LA
+CLIPPERS</t>
+  </si>
+  <si>
+    <t>LOS ANGELES
+LAKERS</t>
+  </si>
+  <si>
+    <t>MEMPHIS
+GRIZZLIES</t>
+  </si>
+  <si>
+    <t>MIAMI
+HEAT</t>
+  </si>
+  <si>
+    <t>MILWAUKEE
+BUCKS</t>
+  </si>
+  <si>
+    <t>MINNESOTA
+TIMBERWOLVES</t>
+  </si>
+  <si>
+    <t>NEW ORLEANS
+PELICANS</t>
+  </si>
+  <si>
+    <t>NEW YORK
+KNICKS</t>
+  </si>
+  <si>
+    <t>OKLAHOMA CITY
+THUNDER</t>
+  </si>
+  <si>
+    <t>ORLANDO
+MAGIC</t>
+  </si>
+  <si>
+    <t>PHILADELPHIA
+76ERS</t>
+  </si>
+  <si>
+    <t>PHOENIX
+SUNS</t>
+  </si>
+  <si>
+    <t>PORTLAND
+TRAIL BLAZERS</t>
+  </si>
+  <si>
+    <t>SACRAMENTO
+KINGS</t>
+  </si>
+  <si>
+    <t>SAN ANTONIO
+SPURS</t>
+  </si>
+  <si>
+    <t>TORONTO
+RAPTORS</t>
+  </si>
+  <si>
+    <t>UTAH
+JAZZ</t>
+  </si>
+  <si>
+    <t>WASHINGTON
+WIZARDS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,9 +275,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -627,7 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA85EE8-E8FA-47DA-86F8-FAC062E4629B}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -647,4 +778,178 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C099605-FEA7-4822-9647-BB6E30494EAA}">
+  <dimension ref="A1:A31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>